<commit_message>
Added PhoneNo Column to parties
</commit_message>
<xml_diff>
--- a/src/assets/excel/Sample Party.xlsx
+++ b/src/assets/excel/Sample Party.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/presidio/Vaish/triplemgarments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/presidio/Vaish/triplemgarments/tripleMDashboard/src/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D00E02-4F8C-A34E-B5EA-57611785BC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDFD874-2C2F-C243-A366-E144A10FD758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{B8AA6C40-226A-D34F-B497-360E1934182C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{B8AA6C40-226A-D34F-B497-360E1934182C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>S.No</t>
   </si>
@@ -63,19 +63,52 @@
   </si>
   <si>
     <t>Someone</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>A.V.K. SRI MURUGALAYA SILKS</t>
+  </si>
+  <si>
+    <t>6/12C,NEAR GOVT GIRLS HIGHER SECONDARY SCHOOL, MALLAMUDRA MAIN ROAD,     (129), MALLASAMUDRAM,NAMAKKAL-637503</t>
+  </si>
+  <si>
+    <t>33BPKPM3070A2ZB</t>
+  </si>
+  <si>
+    <t>ASHWIN SILKS</t>
+  </si>
+  <si>
+    <t>NO:74 B/7,THIRUVANAMALAI MAIN</t>
+  </si>
+  <si>
+    <t>94873 81831  (101)</t>
+  </si>
+  <si>
+    <t>88/89,BAZAAR STREET,</t>
+  </si>
+  <si>
+    <t>33AAMPK2937Q1Z5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,10 +119,34 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -98,8 +155,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,15 +477,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3288DB0F-D8D8-EE48-B159-566BC08794FC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +501,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,8 +518,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>9500977257</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -462,9 +534,52 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3">
+        <v>9998887776</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>